<commit_message>
Return to initial commit
</commit_message>
<xml_diff>
--- a/xlsx_initial/schedule_planning.xlsx
+++ b/xlsx_initial/schedule_planning.xlsx
@@ -2578,10 +2578,10 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B86" sqref="B86"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2762,9 +2762,7 @@
       <c r="C13" s="8">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D13" s="8">
-        <v>0.82291666666666663</v>
-      </c>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">

</xml_diff>